<commit_message>
Design power system circuit with converters
</commit_message>
<xml_diff>
--- a/Electronics/GPIOs data.xlsx
+++ b/Electronics/GPIOs data.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -762,11 +765,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -786,35 +810,42 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1090,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,20 +1137,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1130,12 +1161,12 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1146,12 +1177,12 @@
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1160,10 +1191,10 @@
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1174,10 +1205,10 @@
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1186,266 +1217,266 @@
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="1"/>
       <c r="F14" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="1"/>
       <c r="F16" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="1"/>
       <c r="F17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="1"/>
       <c r="F18" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="1"/>
       <c r="F19" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="1"/>
       <c r="F20" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="1"/>
       <c r="F22" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="1"/>
       <c r="F23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="1"/>
       <c r="F24" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="126" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="6"/>
+      <c r="D25" s="13"/>
       <c r="E25" s="1"/>
       <c r="F25" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="126" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="6"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="1"/>
       <c r="F26" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="14"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -1454,40 +1485,40 @@
       <c r="B29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="7"/>
+      <c r="D29" s="14"/>
       <c r="E29" s="1"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="8"/>
+      <c r="D30" s="15"/>
       <c r="E30" s="1"/>
       <c r="F30" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E31" s="1"/>
@@ -1495,17 +1526,17 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="4" t="s">
         <v>72</v>
       </c>
       <c r="E32" s="1"/>
@@ -1513,17 +1544,17 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="12"/>
+      <c r="D33" s="16"/>
       <c r="E33" s="1"/>
       <c r="F33" s="2" t="s">
         <v>76</v>
@@ -1536,12 +1567,12 @@
       <c r="B34" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="13"/>
+      <c r="D34" s="17"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="4"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -1550,40 +1581,40 @@
       <c r="B35" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="13"/>
+      <c r="D35" s="17"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="4"/>
+      <c r="D36" s="11"/>
       <c r="E36" s="1"/>
       <c r="F36" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="4"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="1"/>
       <c r="F37" s="2" t="s">
         <v>87</v>
@@ -1596,12 +1627,12 @@
       <c r="B38" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="4"/>
+      <c r="D38" s="11"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="14"/>
+      <c r="F38" s="6"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -1610,10 +1641,10 @@
       <c r="B39" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="7"/>
+      <c r="D39" s="14"/>
       <c r="E39" s="1"/>
       <c r="F39" s="2"/>
     </row>
@@ -1624,10 +1655,10 @@
       <c r="B40" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D40" s="7"/>
+      <c r="D40" s="14"/>
       <c r="E40" s="1"/>
       <c r="F40" s="2"/>
     </row>
@@ -1638,24 +1669,29 @@
       <c r="B41" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
       <c r="E41" s="1"/>
       <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
       <c r="E42" s="1"/>
       <c r="F42" s="2"/>
     </row>
+    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="19"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:B1"/>
   <mergeCells count="33">
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="C36:D36"/>
@@ -1670,11 +1706,6 @@
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="F34:F35"/>
     <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:D28"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="A8:A22"/>
@@ -1682,6 +1713,11 @@
     <mergeCell ref="C8:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:D28"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:F3"/>
@@ -1691,6 +1727,12 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
   </mergeCells>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Write down the pins connections for motors
</commit_message>
<xml_diff>
--- a/Electronics/GPIOs data.xlsx
+++ b/Electronics/GPIOs data.xlsx
@@ -4,13 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Draft" sheetId="2" r:id="rId1"/>
+    <sheet name="Raspberry Pi" sheetId="1" r:id="rId2"/>
+    <sheet name="MCP23S17(IC0)" sheetId="3" r:id="rId3"/>
+    <sheet name="74HC4053(IC0)" sheetId="4" r:id="rId4"/>
+    <sheet name="74HC4053(IC1)" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'74HC4053(IC0)'!$A$1:$A$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'74HC4053(IC1)'!$A$1:$A$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Draft!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'MCP23S17(IC0)'!$A$1:$A$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Raspberry Pi'!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="179">
   <si>
     <t>GPIO No</t>
   </si>
@@ -587,6 +595,228 @@
   </si>
   <si>
     <t>Current (mA)</t>
+  </si>
+  <si>
+    <t>GPA 0</t>
+  </si>
+  <si>
+    <t>GPA 1</t>
+  </si>
+  <si>
+    <t>Pin id</t>
+  </si>
+  <si>
+    <t>GPA 2</t>
+  </si>
+  <si>
+    <t>GPA 3</t>
+  </si>
+  <si>
+    <t>GPA 4</t>
+  </si>
+  <si>
+    <t>GPA 5</t>
+  </si>
+  <si>
+    <t>GPA 6</t>
+  </si>
+  <si>
+    <t>GPA 7</t>
+  </si>
+  <si>
+    <t>GPB 0</t>
+  </si>
+  <si>
+    <t>GPB 1</t>
+  </si>
+  <si>
+    <t>GPB 2</t>
+  </si>
+  <si>
+    <t>GPB 3</t>
+  </si>
+  <si>
+    <t>GPB 4</t>
+  </si>
+  <si>
+    <t>GPB 5</t>
+  </si>
+  <si>
+    <t>GPB 6</t>
+  </si>
+  <si>
+    <t>GPB 7</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0) SCK Pin</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0) SO Pin</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0) SI Pin</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0) CS Pin</t>
+  </si>
+  <si>
+    <t>Pins R_EN &amp; L_EN of BTS7960(IC0)</t>
+  </si>
+  <si>
+    <t>Pins R_EN &amp; L_EN of BTS7960(IC1)</t>
+  </si>
+  <si>
+    <t>Pins R_EN &amp; L_EN of BTS7960(IC2)</t>
+  </si>
+  <si>
+    <t>Pins R_EN &amp; L_EN of BTS7960(IC3)</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>GPIO 12 / BCM 10</t>
+  </si>
+  <si>
+    <t>GPIO 13 / BCM 9</t>
+  </si>
+  <si>
+    <t>GPIO 14 / BCM 11</t>
+  </si>
+  <si>
+    <t>GPIO 10 / BCM 8</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>1Y0</t>
+  </si>
+  <si>
+    <t>2Y0</t>
+  </si>
+  <si>
+    <t>3Y0</t>
+  </si>
+  <si>
+    <t>1Y1</t>
+  </si>
+  <si>
+    <t>2Y1</t>
+  </si>
+  <si>
+    <t>3Y1</t>
+  </si>
+  <si>
+    <t>1Z</t>
+  </si>
+  <si>
+    <t>2Z</t>
+  </si>
+  <si>
+    <t>3Z</t>
+  </si>
+  <si>
+    <t>Pin S1 of 74HC4053(IC0)</t>
+  </si>
+  <si>
+    <t>Pin S2 of 74HC4053(IC0)</t>
+  </si>
+  <si>
+    <t>Pin S3 of 74HC4053(IC0)</t>
+  </si>
+  <si>
+    <t>Pin S1 of 74HC4053(IC1)</t>
+  </si>
+  <si>
+    <t>Pin S2 of 74HC4053(IC1)</t>
+  </si>
+  <si>
+    <t>Pin S3 of 74HC4053(IC1)</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0) Pin GPA 0</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0) Pin GPA 1</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0) Pin GPA 2</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0) Pin GPB 0</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0) Pin GPB 1</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0) Pin GPB 2</t>
+  </si>
+  <si>
+    <t>BTS7960(0) Pin RPWM</t>
+  </si>
+  <si>
+    <t>BTS7960(1) Pin RPWM</t>
+  </si>
+  <si>
+    <t>BTS7960(0) Pin LPWM</t>
+  </si>
+  <si>
+    <t>GPIO 23 / BCM 13</t>
+  </si>
+  <si>
+    <t>To 1Z pin of 74HC4053(IC0) for Front Left Motor</t>
+  </si>
+  <si>
+    <t>BTS7960(1) Pin LPWM</t>
+  </si>
+  <si>
+    <t>GPIO 24 / BCM 19</t>
+  </si>
+  <si>
+    <t>To 2Z pin of 74HC4053(IC0) for Front Right Motor</t>
+  </si>
+  <si>
+    <t>BTS7960(3) Pin RPWM</t>
+  </si>
+  <si>
+    <t>BTS7960(3) Pin LPWM</t>
+  </si>
+  <si>
+    <t>To 1Z pin of 74HC4053(IC1) for Rear Left Motor</t>
+  </si>
+  <si>
+    <t>BTS7960(2) Pin RPWM</t>
+  </si>
+  <si>
+    <t>BTS7960(2) Pin LPWM</t>
+  </si>
+  <si>
+    <t>GPIO 1 / BCM 18</t>
+  </si>
+  <si>
+    <t>To 2Z pin of 74HC4053(IC1) for Rear Right Motor</t>
+  </si>
+  <si>
+    <t>GPIO 26 / BCM 12</t>
+  </si>
+  <si>
+    <t>Servo Motor (steering wheel)</t>
   </si>
 </sst>
 </file>
@@ -738,7 +968,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -761,11 +991,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -792,16 +1048,23 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -816,15 +1079,82 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1123,7 +1453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
@@ -1137,558 +1467,558 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="11"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="11"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="11"/>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="13"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="10" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="13"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="13"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="13"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="13"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="14"/>
+      <c r="D27" s="17"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="11"/>
+      <c r="F27" s="16"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="11"/>
+      <c r="F28" s="16"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="14"/>
+      <c r="D29" s="17"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="2"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="15"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="10" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="11" t="s">
         <v>67</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="10" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="11" t="s">
         <v>72</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="10" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="16"/>
+      <c r="D33" s="19"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="17"/>
+      <c r="D34" s="20"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="11"/>
+      <c r="F34" s="16"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="17"/>
+      <c r="D35" s="20"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="11"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="11"/>
+      <c r="D36" s="16"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="10" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="11"/>
+      <c r="D37" s="16"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="11"/>
+      <c r="D38" s="16"/>
       <c r="E38" s="1"/>
       <c r="F38" s="6"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="14"/>
+      <c r="D39" s="17"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="2"/>
+      <c r="F39" s="10"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D40" s="14"/>
+      <c r="D40" s="17"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="2"/>
+      <c r="F40" s="10"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="2"/>
+      <c r="F41" s="10"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="2"/>
+      <c r="F42" s="10"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="19"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1"/>
@@ -1706,6 +2036,11 @@
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="F34:F35"/>
     <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:D28"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="A8:A22"/>
@@ -1713,11 +2048,6 @@
     <mergeCell ref="C8:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:D28"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:F3"/>
@@ -1728,9 +2058,952 @@
     <mergeCell ref="C6:D6"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="25"/>
+    </row>
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="25"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="25"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="25"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="25"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="19"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="25"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="25"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="16"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="15"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B1"/>
+  <mergeCells count="27">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1"/>
+  <conditionalFormatting sqref="A1:A17 A22:A1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="25"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="25"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="25" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="25"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="25" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="25"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1"/>
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Design circuits for water cooling
</commit_message>
<xml_diff>
--- a/Electronics/GPIOs data.xlsx
+++ b/Electronics/GPIOs data.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Draft" sheetId="2" r:id="rId1"/>
     <sheet name="Raspberry Pi" sheetId="1" r:id="rId2"/>
     <sheet name="MCP23S17(IC0)" sheetId="3" r:id="rId3"/>
-    <sheet name="74HC4053(IC0)" sheetId="4" r:id="rId4"/>
-    <sheet name="74HC4053(IC1)" sheetId="6" r:id="rId5"/>
+    <sheet name="MCP23S17(IC1)" sheetId="7" r:id="rId4"/>
+    <sheet name="74HC4053(IC0)" sheetId="4" r:id="rId5"/>
+    <sheet name="74HC4053(IC1)" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'74HC4053(IC0)'!$A$1:$A$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'74HC4053(IC1)'!$A$1:$A$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'74HC4053(IC0)'!$A$1:$A$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'74HC4053(IC1)'!$A$1:$A$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Draft!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'MCP23S17(IC0)'!$A$1:$A$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'MCP23S17(IC1)'!$A$1:$A$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Raspberry Pi'!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="181">
   <si>
     <t>GPIO No</t>
   </si>
@@ -648,18 +650,6 @@
     <t>GPB 7</t>
   </si>
   <si>
-    <t>MCP23S17(IC0) SCK Pin</t>
-  </si>
-  <si>
-    <t>MCP23S17(IC0) SO Pin</t>
-  </si>
-  <si>
-    <t>MCP23S17(IC0) SI Pin</t>
-  </si>
-  <si>
-    <t>MCP23S17(IC0) CS Pin</t>
-  </si>
-  <si>
     <t>Pins R_EN &amp; L_EN of BTS7960(IC0)</t>
   </si>
   <si>
@@ -817,6 +807,24 @@
   </si>
   <si>
     <t>Servo Motor (steering wheel)</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0, IC1) SI Pin</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0, IC1) SO Pin</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0, IC1) SCK Pin</t>
+  </si>
+  <si>
+    <t>MCP23S17(IC0, IC1) CS Pin</t>
+  </si>
+  <si>
+    <t>Pin Input1 of L293D(IC0)</t>
+  </si>
+  <si>
+    <t>Pin Input2 of L293D(IC0)</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1067,6 +1075,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -1079,10 +1096,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1090,9 +1107,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1104,7 +1118,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1453,7 +1477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
@@ -1473,10 +1497,10 @@
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="9" t="s">
         <v>104</v>
       </c>
@@ -1491,12 +1515,12 @@
       <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="24"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="19" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1507,12 +1531,12 @@
       <c r="B3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="24"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="16"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1521,10 +1545,10 @@
       <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="19" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1535,10 +1559,10 @@
       <c r="B5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="16"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
@@ -1547,10 +1571,10 @@
       <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="16"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -1559,164 +1583,164 @@
       <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="1"/>
       <c r="F7" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="1"/>
       <c r="F8" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="1"/>
       <c r="F9" s="10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="1"/>
       <c r="F10" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="1"/>
       <c r="F11" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="1"/>
       <c r="F12" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="1"/>
       <c r="F13" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="1"/>
       <c r="F14" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="1"/>
       <c r="F15" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
       <c r="E16" s="1"/>
       <c r="F16" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="1"/>
       <c r="F17" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="1"/>
       <c r="F18" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="1"/>
       <c r="F19" s="10" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="1"/>
       <c r="F20" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="1"/>
       <c r="F21" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
       <c r="E22" s="1"/>
       <c r="F22" s="10" t="s">
         <v>38</v>
@@ -1729,10 +1753,10 @@
       <c r="B23" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="22"/>
+      <c r="D23" s="24"/>
       <c r="E23" s="1"/>
       <c r="F23" s="10" t="s">
         <v>39</v>
@@ -1745,10 +1769,10 @@
       <c r="B24" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="22"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="1"/>
       <c r="F24" s="10" t="s">
         <v>40</v>
@@ -1761,10 +1785,10 @@
       <c r="B25" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="22"/>
+      <c r="D25" s="24"/>
       <c r="E25" s="1"/>
       <c r="F25" s="10" t="s">
         <v>41</v>
@@ -1777,36 +1801,36 @@
       <c r="B26" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="22"/>
+      <c r="D26" s="24"/>
       <c r="E26" s="1"/>
       <c r="F26" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="17"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="16"/>
+      <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="16"/>
+      <c r="F28" s="19"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
@@ -1815,10 +1839,10 @@
       <c r="B29" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="17"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="1"/>
       <c r="F29" s="10"/>
     </row>
@@ -1829,10 +1853,10 @@
       <c r="B30" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="18"/>
+      <c r="D30" s="21"/>
       <c r="E30" s="1"/>
       <c r="F30" s="10" t="s">
         <v>64</v>
@@ -1881,10 +1905,10 @@
       <c r="B33" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="19"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="1"/>
       <c r="F33" s="10" t="s">
         <v>76</v>
@@ -1897,12 +1921,12 @@
       <c r="B34" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="20"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="16"/>
+      <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
@@ -1911,12 +1935,12 @@
       <c r="B35" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="20"/>
+      <c r="D35" s="23"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="16"/>
+      <c r="F35" s="19"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
@@ -1925,10 +1949,10 @@
       <c r="B36" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="16"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="1"/>
       <c r="F36" s="10" t="s">
         <v>86</v>
@@ -1941,10 +1965,10 @@
       <c r="B37" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="16"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="1"/>
       <c r="F37" s="10" t="s">
         <v>87</v>
@@ -1957,10 +1981,10 @@
       <c r="B38" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="16"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="1"/>
       <c r="F38" s="6"/>
     </row>
@@ -1971,10 +1995,10 @@
       <c r="B39" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="17"/>
+      <c r="D39" s="20"/>
       <c r="E39" s="1"/>
       <c r="F39" s="10"/>
     </row>
@@ -1985,10 +2009,10 @@
       <c r="B40" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="D40" s="17"/>
+      <c r="D40" s="20"/>
       <c r="E40" s="1"/>
       <c r="F40" s="10"/>
     </row>
@@ -1999,8 +2023,8 @@
       <c r="B41" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="1"/>
       <c r="F41" s="10"/>
     </row>
@@ -2011,8 +2035,8 @@
       <c r="B42" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
       <c r="E42" s="1"/>
       <c r="F42" s="10"/>
     </row>
@@ -2023,31 +2047,6 @@
   </sheetData>
   <autoFilter ref="A1:B1"/>
   <mergeCells count="33">
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:A22"/>
-    <mergeCell ref="B8:B22"/>
-    <mergeCell ref="C8:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:F3"/>
@@ -2056,12 +2055,37 @@
     <mergeCell ref="F4:F6"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:A22"/>
+    <mergeCell ref="B8:B22"/>
+    <mergeCell ref="C8:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2072,8 +2096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,10 +2116,10 @@
       <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="7" t="s">
         <v>104</v>
       </c>
@@ -2110,12 +2134,12 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="24"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="25"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2124,12 +2148,12 @@
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="24"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="25"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2138,10 +2162,10 @@
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="25"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -2150,10 +2174,10 @@
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="25"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -2162,10 +2186,10 @@
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="25"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -2174,27 +2198,27 @@
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="27"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2204,13 +2228,13 @@
       <c r="B9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2220,13 +2244,13 @@
       <c r="B10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2236,13 +2260,13 @@
       <c r="B11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="22"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
-        <v>125</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2252,34 +2276,34 @@
       <c r="B12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="1"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="17"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="25"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="25"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -2288,10 +2312,10 @@
       <c r="B15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="17"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2"/>
     </row>
@@ -2302,13 +2326,13 @@
       <c r="B16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="1"/>
       <c r="F16" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -2326,7 +2350,7 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="10" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -2344,7 +2368,7 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="10" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -2354,13 +2378,13 @@
       <c r="B19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="1"/>
       <c r="F19" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2370,12 +2394,12 @@
       <c r="B20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="20"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="25"/>
+      <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -2384,12 +2408,12 @@
       <c r="B21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="20"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="25"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -2398,10 +2422,10 @@
       <c r="B22" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="16"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
     </row>
@@ -2412,10 +2436,10 @@
       <c r="B23" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="16"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
     </row>
@@ -2426,10 +2450,10 @@
       <c r="B24" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="16"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="1"/>
       <c r="F24" s="6"/>
     </row>
@@ -2440,10 +2464,10 @@
       <c r="B25" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="17"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="1"/>
       <c r="F25" s="2"/>
     </row>
@@ -2454,10 +2478,10 @@
       <c r="B26" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="17"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="1"/>
       <c r="F26" s="2"/>
     </row>
@@ -2468,8 +2492,8 @@
       <c r="B27" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="1"/>
       <c r="F27" s="2"/>
     </row>
@@ -2480,8 +2504,8 @@
       <c r="B28" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="1"/>
       <c r="F28" s="2"/>
     </row>
@@ -2492,26 +2516,6 @@
   </sheetData>
   <autoFilter ref="A1:B1"/>
   <mergeCells count="27">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
@@ -2519,12 +2523,32 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2562,8 +2586,8 @@
         <v>105</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="25" t="s">
-        <v>150</v>
+      <c r="C2" s="18" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2571,8 +2595,8 @@
         <v>106</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="25" t="s">
-        <v>151</v>
+      <c r="C3" s="18" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2580,8 +2604,8 @@
         <v>108</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="25" t="s">
-        <v>152</v>
+      <c r="C4" s="18" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2589,8 +2613,8 @@
         <v>109</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="25" t="s">
-        <v>126</v>
+      <c r="C5" s="18" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2598,8 +2622,8 @@
         <v>110</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="25" t="s">
-        <v>127</v>
+      <c r="C6" s="18" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2628,8 +2652,8 @@
         <v>114</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="25" t="s">
-        <v>153</v>
+      <c r="C10" s="18" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2637,8 +2661,8 @@
         <v>115</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="25" t="s">
-        <v>154</v>
+      <c r="C11" s="18" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2646,8 +2670,8 @@
         <v>116</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="25" t="s">
-        <v>155</v>
+      <c r="C12" s="18" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2655,8 +2679,8 @@
         <v>117</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="25" t="s">
-        <v>128</v>
+      <c r="C13" s="18" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2664,8 +2688,8 @@
         <v>118</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="25" t="s">
-        <v>129</v>
+      <c r="C14" s="18" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2691,44 +2715,44 @@
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="10" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="10" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="10" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1"/>
   <conditionalFormatting sqref="A1:A17 A22:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2736,6 +2760,194 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="18"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="18"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="18"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="16"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="16"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="16"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="18"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="18"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="18"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="18"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="18"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="16"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1"/>
+  <conditionalFormatting sqref="A1:A17 A22:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -2763,117 +2975,117 @@
     </row>
     <row r="2" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="25" t="s">
-        <v>156</v>
+      <c r="C2" s="18" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="25" t="s">
-        <v>157</v>
+      <c r="C3" s="18" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="25" t="s">
-        <v>158</v>
+      <c r="C4" s="18" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="25" t="s">
-        <v>162</v>
+      <c r="C5" s="18" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="25" t="s">
-        <v>163</v>
+      <c r="C6" s="18" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="25" t="s">
-        <v>164</v>
+      <c r="C8" s="18" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="25" t="s">
-        <v>167</v>
+      <c r="C9" s="18" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="25"/>
+      <c r="C10" s="18"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="25" t="s">
-        <v>165</v>
+      <c r="C11" s="18" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="25" t="s">
-        <v>168</v>
+      <c r="C12" s="18" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="25"/>
+      <c r="C13" s="18"/>
     </row>
   </sheetData>
   <autoFilter ref="A1"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -2901,110 +3113,110 @@
     </row>
     <row r="2" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="25" t="s">
-        <v>159</v>
+      <c r="C2" s="18" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="25" t="s">
-        <v>160</v>
+      <c r="C3" s="18" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="25" t="s">
-        <v>161</v>
+      <c r="C4" s="18" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="25" t="s">
-        <v>173</v>
+      <c r="C5" s="18" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="25" t="s">
-        <v>170</v>
+      <c r="C6" s="18" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="25" t="s">
-        <v>174</v>
+      <c r="C8" s="18" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="25" t="s">
-        <v>171</v>
+      <c r="C9" s="18" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="25"/>
+      <c r="C10" s="18"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="25" t="s">
-        <v>175</v>
+      <c r="C11" s="18" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="25" t="s">
-        <v>177</v>
+      <c r="C12" s="18" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="25"/>
+      <c r="C13" s="18"/>
     </row>
   </sheetData>
   <autoFilter ref="A1"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Improve electronics data stats
</commit_message>
<xml_diff>
--- a/Electronics/GPIOs data.xlsx
+++ b/Electronics/GPIOs data.xlsx
@@ -2026,7 +2026,7 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -2079,8 +2079,8 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="13" t="n">
-        <f aca="false">(3.3/5700)*1000</f>
-        <v>0.578947368421053</v>
+        <f aca="false">(3.3/5540)*1000</f>
+        <v>0.595667870036101</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>108</v>
@@ -2512,7 +2512,7 @@
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="13" t="n">
         <f aca="false">SUM(E2:E28)</f>
-        <v>0.578947368421053</v>
+        <v>0.595667870036101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>